<commit_message>
Refining and plotting final metrics.
</commit_message>
<xml_diff>
--- a/data/metrics/sens.filt.2020-12-23.xlsx
+++ b/data/metrics/sens.filt.2020-12-23.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,19 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\LGSS_scripting\lgss\data\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{69A985E4-CBAF-4AF3-B1BD-1D1E47781C23}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5803EC0E-D2EA-435F-B29D-9A613B791C12}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="10690" windowWidth="19420" windowHeight="11020"/>
+    <workbookView xWindow="-110" yWindow="10690" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sens.filt.2020-12-23" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="75">
   <si>
     <t>metric</t>
   </si>
@@ -136,9 +144,6 @@
     <t>notes</t>
   </si>
   <si>
-    <t xml:space="preserve">Only ffg metric </t>
-  </si>
-  <si>
     <t>dominance</t>
   </si>
   <si>
@@ -178,31 +183,82 @@
     <t>Keep? (or cote)</t>
   </si>
   <si>
-    <t>same as EPT</t>
-  </si>
-  <si>
     <t>low DE</t>
   </si>
   <si>
     <t>or intol_facul?</t>
   </si>
   <si>
-    <t>or intolerant?</t>
-  </si>
-  <si>
-    <t>best DE</t>
-  </si>
-  <si>
-    <t>or ept?</t>
-  </si>
-  <si>
-    <t>or ttaxa? This has higher DE.</t>
+    <t>sub for ept above?</t>
+  </si>
+  <si>
+    <t>pct_rich_ttaxa_cte</t>
+  </si>
+  <si>
+    <t>shannon_ttaxa_coe</t>
+  </si>
+  <si>
+    <t>shannon_ttaxa_cote</t>
+  </si>
+  <si>
+    <t>shannon_ttaxa_cte</t>
+  </si>
+  <si>
+    <t>shannon_ttaxa_potec</t>
+  </si>
+  <si>
+    <t>shannon_ttaxa_toe</t>
+  </si>
+  <si>
+    <t>new</t>
+  </si>
+  <si>
+    <t>simpson_ttaxa_coe</t>
+  </si>
+  <si>
+    <t>simpson_ttaxa_cote</t>
+  </si>
+  <si>
+    <t>simpson_ttaxa_potec</t>
+  </si>
+  <si>
+    <t>simpson_ttaxa_toe</t>
+  </si>
+  <si>
+    <t>Low DE but only passing ffg metric.</t>
+  </si>
+  <si>
+    <t>Keep? (or potec)</t>
+  </si>
+  <si>
+    <t>new; best DE. Or match with other cote metric?</t>
+  </si>
+  <si>
+    <t>new; not best but matches w other cote metric.</t>
+  </si>
+  <si>
+    <t>or ept/et?</t>
+  </si>
+  <si>
+    <t>same as EPT. P may not tell us anything.</t>
+  </si>
+  <si>
+    <t>Same DE as et, but results in fewer 0 output scores.</t>
+  </si>
+  <si>
+    <t>Same DE as cote, but maybe result in fewer 0 output scores.</t>
+  </si>
+  <si>
+    <t>Same DE as intol, but results in fewer 0 output scores.</t>
+  </si>
+  <si>
+    <t>Removed bc high corr w rich_taxa_et and shannon_taxa_toe.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -339,7 +395,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -528,6 +584,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -692,13 +766,16 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1053,11 +1130,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:XFD16"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1065,13 +1142,13 @@
     <col min="1" max="1" width="24.85546875" customWidth="1"/>
     <col min="2" max="2" width="24.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.140625" customWidth="1"/>
-    <col min="4" max="4" width="31.28515625" customWidth="1"/>
+    <col min="4" max="4" width="47.5703125" customWidth="1"/>
     <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
     <col min="7" max="10" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>36</v>
       </c>
@@ -1079,7 +1156,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>37</v>
@@ -1103,9 +1180,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B2" t="s">
         <v>30</v>
@@ -1132,9 +1209,9 @@
         <v>68.870967741935502</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B3" t="s">
         <v>31</v>
@@ -1161,9 +1238,9 @@
         <v>67.204301075268802</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>25</v>
@@ -1190,9 +1267,9 @@
         <v>72.096774193548399</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B5" t="s">
         <v>26</v>
@@ -1201,7 +1278,7 @@
         <v>33</v>
       </c>
       <c r="D5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E5" t="s">
         <v>24</v>
@@ -1222,44 +1299,51 @@
         <v>70.483870967741893</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>48</v>
-      </c>
-      <c r="B6" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+      <c r="G6">
+        <v>18.452380952380999</v>
+      </c>
+      <c r="H6">
+        <v>70</v>
+      </c>
+      <c r="I6">
+        <v>19.5299145299145</v>
+      </c>
+      <c r="J6">
+        <v>70.483870967741893</v>
+      </c>
+      <c r="K6" s="4"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6">
-        <v>3</v>
-      </c>
-      <c r="G6">
-        <v>22.835497835497801</v>
-      </c>
-      <c r="H6">
-        <v>80</v>
-      </c>
-      <c r="I6">
-        <v>21.506513409961698</v>
-      </c>
-      <c r="J6">
-        <v>75.430107526881699</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>48</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>51</v>
+      <c r="C7" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="D7" t="s">
+        <v>74</v>
       </c>
       <c r="E7" t="s">
         <v>8</v>
@@ -1274,24 +1358,24 @@
         <v>80</v>
       </c>
       <c r="I7">
-        <v>21.269509981851201</v>
+        <v>21.506513409961698</v>
       </c>
       <c r="J7">
-        <v>80.268817204301101</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+        <v>75.430107526881699</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>48</v>
-      </c>
-      <c r="B8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" t="s">
-        <v>33</v>
+        <v>47</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>50</v>
       </c>
       <c r="D8" t="s">
-        <v>50</v>
+        <v>72</v>
       </c>
       <c r="E8" t="s">
         <v>8</v>
@@ -1300,30 +1384,30 @@
         <v>3</v>
       </c>
       <c r="G8">
-        <v>15.470494417862801</v>
+        <v>22.835497835497801</v>
       </c>
       <c r="H8">
-        <v>76.6666666666667</v>
+        <v>80</v>
       </c>
       <c r="I8">
-        <v>15.6785714285714</v>
+        <v>21.269509981851201</v>
       </c>
       <c r="J8">
-        <v>75.430107526881699</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+        <v>80.268817204301101</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C9" t="s">
         <v>33</v>
       </c>
       <c r="D9" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E9" t="s">
         <v>8</v>
@@ -1332,30 +1416,30 @@
         <v>3</v>
       </c>
       <c r="G9">
-        <v>15.5</v>
+        <v>15.470494417862801</v>
       </c>
       <c r="H9">
-        <v>80</v>
+        <v>76.6666666666667</v>
       </c>
       <c r="I9">
-        <v>15.14</v>
+        <v>15.6785714285714</v>
       </c>
       <c r="J9">
-        <v>77.096774193548399</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+        <v>75.430107526881699</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C10" t="s">
         <v>33</v>
       </c>
       <c r="D10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E10" t="s">
         <v>8</v>
@@ -1364,30 +1448,30 @@
         <v>3</v>
       </c>
       <c r="G10">
-        <v>30</v>
+        <v>15.5</v>
       </c>
       <c r="H10">
         <v>80</v>
       </c>
       <c r="I10">
-        <v>29.88</v>
+        <v>15.14</v>
       </c>
       <c r="J10">
-        <v>78.709677419354804</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+        <v>77.096774193548399</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>41</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>57</v>
+        <v>40</v>
+      </c>
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" t="s">
+        <v>45</v>
       </c>
       <c r="E11" t="s">
         <v>8</v>
@@ -1396,62 +1480,62 @@
         <v>3</v>
       </c>
       <c r="G11">
+        <v>30</v>
+      </c>
+      <c r="H11">
+        <v>80</v>
+      </c>
+      <c r="I11">
+        <v>29.88</v>
+      </c>
+      <c r="J11">
+        <v>78.709677419354804</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12">
+        <v>3</v>
+      </c>
+      <c r="G12">
         <v>30.5</v>
       </c>
-      <c r="H11">
+      <c r="H12">
         <v>83.3333333333333</v>
       </c>
-      <c r="I11">
+      <c r="I12">
         <v>29.6</v>
       </c>
-      <c r="J11">
+      <c r="J12">
         <v>80.322580645161295</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>41</v>
-      </c>
-      <c r="B12" t="s">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" t="s">
         <v>44</v>
-      </c>
-      <c r="C12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D12" t="s">
-        <v>45</v>
-      </c>
-      <c r="E12" t="s">
-        <v>8</v>
-      </c>
-      <c r="F12">
-        <v>2</v>
-      </c>
-      <c r="G12">
-        <v>7</v>
-      </c>
-      <c r="H12">
-        <v>66.6666666666667</v>
-      </c>
-      <c r="I12">
-        <v>7</v>
-      </c>
-      <c r="J12">
-        <v>65.591397849462396</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>41</v>
-      </c>
-      <c r="B13" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13" t="s">
-        <v>33</v>
-      </c>
-      <c r="D13" t="s">
-        <v>53</v>
       </c>
       <c r="E13" t="s">
         <v>8</v>
@@ -1460,62 +1544,62 @@
         <v>2</v>
       </c>
       <c r="G13">
-        <v>11.5</v>
+        <v>7</v>
       </c>
       <c r="H13">
         <v>66.6666666666667</v>
       </c>
       <c r="I13">
+        <v>7</v>
+      </c>
+      <c r="J13">
+        <v>65.591397849462396</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" t="s">
+        <v>51</v>
+      </c>
+      <c r="E14" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14">
+        <v>2</v>
+      </c>
+      <c r="G14">
+        <v>11.5</v>
+      </c>
+      <c r="H14">
+        <v>66.6666666666667</v>
+      </c>
+      <c r="I14">
         <v>11.68</v>
       </c>
-      <c r="J13">
+      <c r="J14">
         <v>70.430107526881699</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>41</v>
-      </c>
-      <c r="B14" s="3" t="s">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D14" t="s">
-        <v>58</v>
-      </c>
-      <c r="E14" t="s">
-        <v>8</v>
-      </c>
-      <c r="F14">
-        <v>3</v>
-      </c>
-      <c r="G14">
-        <v>3.5</v>
-      </c>
-      <c r="H14">
-        <v>86.6666666666667</v>
-      </c>
-      <c r="I14">
-        <v>2.6</v>
-      </c>
-      <c r="J14">
-        <v>83.494623655913998</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>41</v>
-      </c>
-      <c r="B15" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15" t="s">
-        <v>33</v>
+      <c r="C15" s="7" t="s">
+        <v>34</v>
       </c>
       <c r="D15" t="s">
-        <v>52</v>
+        <v>71</v>
       </c>
       <c r="E15" t="s">
         <v>8</v>
@@ -1536,47 +1620,50 @@
         <v>83.494623655913998</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>43</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>35</v>
+        <v>40</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>53</v>
       </c>
       <c r="D16" t="s">
-        <v>38</v>
+        <v>70</v>
       </c>
       <c r="E16" t="s">
         <v>8</v>
       </c>
       <c r="F16">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G16">
-        <v>10.5</v>
+        <v>3.5</v>
       </c>
       <c r="H16">
-        <v>66.6666666666667</v>
+        <v>86.6666666666667</v>
       </c>
       <c r="I16">
-        <v>11.4</v>
+        <v>2.6</v>
       </c>
       <c r="J16">
-        <v>65.591397849462396</v>
+        <v>83.494623655913998</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>47</v>
-      </c>
-      <c r="B17" t="s">
-        <v>27</v>
-      </c>
-      <c r="C17" t="s">
-        <v>33</v>
+        <v>42</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" t="s">
+        <v>65</v>
       </c>
       <c r="E17" t="s">
         <v>8</v>
@@ -1585,62 +1672,59 @@
         <v>2</v>
       </c>
       <c r="G17">
-        <v>2.8084333787031799</v>
+        <v>10.5</v>
       </c>
       <c r="H17">
         <v>66.6666666666667</v>
       </c>
       <c r="I17">
-        <v>2.9091287722608201</v>
+        <v>11.4</v>
       </c>
       <c r="J17">
-        <v>70.483870967741893</v>
+        <v>65.591397849462396</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>47</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D18" t="s">
-        <v>55</v>
+        <v>46</v>
+      </c>
+      <c r="B18" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" t="s">
+        <v>33</v>
       </c>
       <c r="E18" t="s">
         <v>8</v>
       </c>
       <c r="F18">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G18">
-        <v>19</v>
+        <v>2.8084333787031799</v>
       </c>
       <c r="H18">
-        <v>76.6666666666667</v>
+        <v>66.6666666666667</v>
       </c>
       <c r="I18">
-        <v>18.86</v>
+        <v>2.9091287722608201</v>
       </c>
       <c r="J18">
-        <v>77.043010752688204</v>
+        <v>70.483870967741893</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>47</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>35</v>
+        <v>46</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>34</v>
       </c>
       <c r="D19" t="s">
-        <v>54</v>
+        <v>73</v>
       </c>
       <c r="E19" t="s">
         <v>8</v>
@@ -1649,13 +1733,13 @@
         <v>3</v>
       </c>
       <c r="G19">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="H19">
         <v>76.6666666666667</v>
       </c>
       <c r="I19">
-        <v>2.46</v>
+        <v>18.86</v>
       </c>
       <c r="J19">
         <v>77.043010752688204</v>
@@ -1663,74 +1747,74 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>47</v>
-      </c>
-      <c r="B20" t="s">
-        <v>21</v>
-      </c>
-      <c r="C20" t="s">
-        <v>33</v>
+        <v>46</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" t="s">
+        <v>52</v>
       </c>
       <c r="E20" t="s">
         <v>8</v>
       </c>
       <c r="F20">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G20">
-        <v>2.8742545493052498</v>
+        <v>3</v>
       </c>
       <c r="H20">
-        <v>73.3333333333333</v>
+        <v>76.6666666666667</v>
       </c>
       <c r="I20">
-        <v>2.8900060206038201</v>
+        <v>2.46</v>
       </c>
       <c r="J20">
-        <v>73.763440860214999</v>
+        <v>77.043010752688204</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>40</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D21" t="s">
-        <v>56</v>
+        <v>46</v>
+      </c>
+      <c r="B21" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" t="s">
+        <v>33</v>
       </c>
       <c r="E21" t="s">
         <v>8</v>
       </c>
       <c r="F21">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G21">
-        <v>12.802199860946899</v>
+        <v>2.8742545493052498</v>
       </c>
       <c r="H21">
-        <v>83.3333333333333</v>
+        <v>73.3333333333333</v>
       </c>
       <c r="I21">
-        <v>12.1603274157769</v>
+        <v>2.8900060206038201</v>
       </c>
       <c r="J21">
-        <v>81.989247311827995</v>
+        <v>73.763440860214999</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>40</v>
-      </c>
-      <c r="B22" t="s">
-        <v>11</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>33</v>
+        <v>39</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="E22" t="s">
         <v>8</v>
@@ -1739,24 +1823,24 @@
         <v>3</v>
       </c>
       <c r="G22">
-        <v>2.1485946181198501</v>
+        <v>12.802199860946899</v>
       </c>
       <c r="H22">
-        <v>80</v>
+        <v>83.3333333333333</v>
       </c>
       <c r="I22">
-        <v>2.0499744890133198</v>
+        <v>12.1603274157769</v>
       </c>
       <c r="J22">
-        <v>80.322580645161295</v>
+        <v>81.989247311827995</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B23" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>33</v>
@@ -1765,27 +1849,27 @@
         <v>8</v>
       </c>
       <c r="F23">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G23">
-        <v>3.5195695769510902</v>
+        <v>2.1485946181198501</v>
       </c>
       <c r="H23">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="I23">
-        <v>3.6086681021069298</v>
+        <v>2.0499744890133198</v>
       </c>
       <c r="J23">
-        <v>72.150537634408593</v>
+        <v>80.322580645161295</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B24" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>33</v>
@@ -1794,27 +1878,27 @@
         <v>8</v>
       </c>
       <c r="F24">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G24">
-        <v>1.78284002465393</v>
+        <v>3.5195695769510902</v>
       </c>
       <c r="H24">
-        <v>76.6666666666667</v>
+        <v>70</v>
       </c>
       <c r="I24">
-        <v>1.79280681362995</v>
+        <v>3.6086681021069298</v>
       </c>
       <c r="J24">
-        <v>77.096774193548399</v>
+        <v>72.150537634408593</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B25" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>33</v>
@@ -1823,55 +1907,375 @@
         <v>8</v>
       </c>
       <c r="F25">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G25">
-        <v>3.4424427630108601</v>
+        <v>1.78284002465393</v>
       </c>
       <c r="H25">
-        <v>70</v>
+        <v>76.6666666666667</v>
       </c>
       <c r="I25">
-        <v>3.4442082477334099</v>
+        <v>1.79280681362995</v>
       </c>
       <c r="J25">
-        <v>70.483870967741893</v>
+        <v>77.096774193548399</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B26" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>33</v>
       </c>
       <c r="E26" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="F26">
         <v>2</v>
       </c>
       <c r="G26">
-        <v>0.371111111111111</v>
+        <v>3.4424427630108601</v>
       </c>
       <c r="H26">
         <v>70</v>
       </c>
       <c r="I26">
+        <v>3.4442082477334099</v>
+      </c>
+      <c r="J26">
+        <v>70.483870967741893</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>39</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F27" s="4">
+        <v>3</v>
+      </c>
+      <c r="G27" s="4">
+        <v>1.8373207647735701</v>
+      </c>
+      <c r="H27" s="4">
+        <v>76.6666666666667</v>
+      </c>
+      <c r="I27" s="4">
+        <v>1.8155980723852001</v>
+      </c>
+      <c r="J27" s="4">
+        <v>77.043010752688204</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>39</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F28" s="4">
+        <v>3</v>
+      </c>
+      <c r="G28" s="4">
+        <v>2.1209372298772502</v>
+      </c>
+      <c r="H28" s="4">
+        <v>86.6666666666667</v>
+      </c>
+      <c r="I28" s="4">
+        <v>1.8608292713544801</v>
+      </c>
+      <c r="J28" s="4">
+        <v>80.322580645161295</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>39</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F29" s="4">
+        <v>3</v>
+      </c>
+      <c r="G29" s="4">
+        <v>1.8528303225668401</v>
+      </c>
+      <c r="H29" s="4">
+        <v>83.3333333333333</v>
+      </c>
+      <c r="I29" s="4">
+        <v>1.6145410757637799</v>
+      </c>
+      <c r="J29" s="4">
+        <v>83.602150537634401</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>39</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F30" s="4">
+        <v>3</v>
+      </c>
+      <c r="G30" s="4">
+        <v>2.1209372298772502</v>
+      </c>
+      <c r="H30" s="4">
+        <v>86.6666666666667</v>
+      </c>
+      <c r="I30" s="4">
+        <v>1.9267486932729301</v>
+      </c>
+      <c r="J30" s="4">
+        <v>81.989247311827995</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>39</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F31" s="4">
+        <v>3</v>
+      </c>
+      <c r="G31" s="4">
+        <v>1.75286296841039</v>
+      </c>
+      <c r="H31" s="6">
+        <v>90</v>
+      </c>
+      <c r="I31" s="4">
+        <v>1.5638554017667201</v>
+      </c>
+      <c r="J31" s="4">
+        <v>88.548387096774206</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>39</v>
+      </c>
+      <c r="B32" t="s">
+        <v>23</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E32" t="s">
+        <v>24</v>
+      </c>
+      <c r="F32">
+        <v>2</v>
+      </c>
+      <c r="G32">
+        <v>0.371111111111111</v>
+      </c>
+      <c r="H32">
+        <v>70</v>
+      </c>
+      <c r="I32">
         <v>0.33212144116906001</v>
       </c>
-      <c r="J26">
+      <c r="J32">
         <v>72.150537634408593</v>
       </c>
     </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>39</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F33" s="4">
+        <v>2</v>
+      </c>
+      <c r="G33" s="4">
+        <v>0.34647433758789498</v>
+      </c>
+      <c r="H33" s="4">
+        <v>70</v>
+      </c>
+      <c r="I33" s="4">
+        <v>0.32888888888888901</v>
+      </c>
+      <c r="J33" s="4">
+        <v>72.150537634408593</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>39</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F34" s="4">
+        <v>3</v>
+      </c>
+      <c r="G34" s="4">
+        <v>0.30845463137996199</v>
+      </c>
+      <c r="H34" s="4">
+        <v>80</v>
+      </c>
+      <c r="I34" s="4">
+        <v>0.32451272360796202</v>
+      </c>
+      <c r="J34" s="4">
+        <v>78.655913978494596</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>39</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F35" s="4">
+        <v>3</v>
+      </c>
+      <c r="G35" s="4">
+        <v>0.29138888888888897</v>
+      </c>
+      <c r="H35" s="4">
+        <v>80</v>
+      </c>
+      <c r="I35" s="4">
+        <v>0.307936157682832</v>
+      </c>
+      <c r="J35" s="4">
+        <v>78.709677419354804</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>39</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F36" s="4">
+        <v>2</v>
+      </c>
+      <c r="G36" s="4">
+        <v>0.33693771626297597</v>
+      </c>
+      <c r="H36" s="4">
+        <v>70</v>
+      </c>
+      <c r="I36" s="4">
+        <v>0.29854600560856298</v>
+      </c>
+      <c r="J36" s="4">
+        <v>70.483870967741893</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D37" s="4"/>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:J26">
-    <sortCondition ref="B2:B26"/>
-    <sortCondition ref="H2:H26"/>
-    <sortCondition ref="F2:F26"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:J32">
+    <sortCondition ref="B2:B32"/>
+    <sortCondition ref="H2:H32"/>
+    <sortCondition ref="F2:F32"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Move sample taxa prep from metrics Rmd to bugs Rmd. Change "unidentified" to "undetermined" in taxa_fill function (to match existing master taxa recs). Update PMA numbers base on new training subset (unknown why different!). Create new bug matrix using species (taxa_fill) for ordination later.
</commit_message>
<xml_diff>
--- a/data/metrics/sens.filt.2020-12-23.xlsx
+++ b/data/metrics/sens.filt.2020-12-23.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\LGSS_scripting\lgss\data\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5803EC0E-D2EA-435F-B29D-9A613B791C12}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E1717A1-FE1F-4F66-BCC7-0BE513554C6F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="10690" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sens.filt.2020-12-23" sheetId="1" r:id="rId1"/>
+    <sheet name="output comparison" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="86">
   <si>
     <t>metric</t>
   </si>
@@ -253,6 +254,39 @@
   </si>
   <si>
     <t>Removed bc high corr w rich_taxa_et and shannon_taxa_toe.</t>
+  </si>
+  <si>
+    <t>rich_ttaxa_toe</t>
+  </si>
+  <si>
+    <t>rich_ttaxa_cot</t>
+  </si>
+  <si>
+    <t>pct_rich_ttaxa_insecta</t>
+  </si>
+  <si>
+    <t>pct_rich_ttaxa_coe</t>
+  </si>
+  <si>
+    <t>rich_ttaxa_insecta</t>
+  </si>
+  <si>
+    <t>rich_ttaxa_facultative</t>
+  </si>
+  <si>
+    <t>rich_ttaxa_coleoptera</t>
+  </si>
+  <si>
+    <t>rich_ttaxa_scraper</t>
+  </si>
+  <si>
+    <t>pct_rich_ttaxa_cot</t>
+  </si>
+  <si>
+    <t>pct_gatherer</t>
+  </si>
+  <si>
+    <t>metric_2020-01-05</t>
   </si>
 </sst>
 </file>
@@ -1134,7 +1168,7 @@
   <dimension ref="A1:K37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2279,4 +2313,334 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E705C07-8672-4EBC-939E-16CB451BAB02}">
+  <dimension ref="A1:C36"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="8"/>
+      <c r="C7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="5"/>
+      <c r="C12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="7"/>
+      <c r="C15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="5"/>
+      <c r="C16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="3"/>
+      <c r="C17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="7"/>
+      <c r="C19" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="5"/>
+      <c r="C20" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="5"/>
+      <c r="C22" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C23" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>16</v>
+      </c>
+      <c r="C24" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C25" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C26" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" s="4"/>
+      <c r="C27" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" s="4"/>
+      <c r="C28" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>21</v>
+      </c>
+      <c r="B29" s="4"/>
+      <c r="C29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B30" s="4"/>
+      <c r="C30" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B31" s="6"/>
+      <c r="C31" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C32" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>23</v>
+      </c>
+      <c r="B33" s="4"/>
+      <c r="C33" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B34" s="4"/>
+      <c r="C34" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B35" s="4"/>
+      <c r="C35" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B36" s="4"/>
+      <c r="C36" t="s">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="F2:F36">
+    <sortCondition ref="F4"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Misc updates from running new subsample. Outputs.
</commit_message>
<xml_diff>
--- a/data/metrics/sens.filt.2020-12-23.xlsx
+++ b/data/metrics/sens.filt.2020-12-23.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\LGSS_scripting\lgss\data\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E1717A1-FE1F-4F66-BCC7-0BE513554C6F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BE88A0F-254C-4E00-8DFA-FDB261F97067}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="10690" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-5895" yWindow="3720" windowWidth="12945" windowHeight="15300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sens.filt.2020-12-23" sheetId="1" r:id="rId1"/>
@@ -226,9 +226,6 @@
     <t>simpson_ttaxa_toe</t>
   </si>
   <si>
-    <t>Low DE but only passing ffg metric.</t>
-  </si>
-  <si>
     <t>Keep? (or potec)</t>
   </si>
   <si>
@@ -287,6 +284,9 @@
   </si>
   <si>
     <t>metric_2020-01-05</t>
+  </si>
+  <si>
+    <t>Low DE but only passing ffg metric. Oppposite response from rich_ttaxa_gatherer in first run!</t>
   </si>
 </sst>
 </file>
@@ -800,7 +800,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -810,6 +810,7 @@
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1168,7 +1169,7 @@
   <dimension ref="A1:K37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="B4" sqref="B4:H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1374,10 +1375,10 @@
         <v>19</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E7" t="s">
         <v>8</v>
@@ -1409,7 +1410,7 @@
         <v>50</v>
       </c>
       <c r="D8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E8" t="s">
         <v>8</v>
@@ -1537,7 +1538,7 @@
         <v>35</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E12" t="s">
         <v>8</v>
@@ -1633,7 +1634,7 @@
         <v>34</v>
       </c>
       <c r="D15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E15" t="s">
         <v>8</v>
@@ -1665,7 +1666,7 @@
         <v>53</v>
       </c>
       <c r="D16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E16" t="s">
         <v>8</v>
@@ -1690,14 +1691,14 @@
       <c r="A17" t="s">
         <v>42</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="9" t="s">
         <v>32</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>34</v>
       </c>
       <c r="D17" t="s">
-        <v>65</v>
+        <v>85</v>
       </c>
       <c r="E17" t="s">
         <v>8</v>
@@ -1758,7 +1759,7 @@
         <v>34</v>
       </c>
       <c r="D19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E19" t="s">
         <v>8</v>
@@ -2028,7 +2029,7 @@
         <v>33</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E28" s="4" t="s">
         <v>8</v>
@@ -2124,7 +2125,7 @@
         <v>34</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E31" s="4" t="s">
         <v>8</v>
@@ -2335,7 +2336,7 @@
       </c>
       <c r="B1" s="1"/>
       <c r="C1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -2376,7 +2377,7 @@
         <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -2385,7 +2386,7 @@
       </c>
       <c r="B7" s="8"/>
       <c r="C7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -2394,7 +2395,7 @@
       </c>
       <c r="B8" s="5"/>
       <c r="C8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -2418,7 +2419,7 @@
         <v>20</v>
       </c>
       <c r="C11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -2487,7 +2488,7 @@
       </c>
       <c r="B19" s="7"/>
       <c r="C19" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -2496,7 +2497,7 @@
       </c>
       <c r="B20" s="5"/>
       <c r="C20" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -2504,7 +2505,7 @@
         <v>18</v>
       </c>
       <c r="C21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -2513,7 +2514,7 @@
       </c>
       <c r="B22" s="5"/>
       <c r="C22" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -2529,7 +2530,7 @@
         <v>16</v>
       </c>
       <c r="C24" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -2537,7 +2538,7 @@
         <v>56</v>
       </c>
       <c r="C25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Rerunning metrics with new subsample created by set.seed(80) after R studio update.
</commit_message>
<xml_diff>
--- a/data/metrics/sens.filt.2020-12-23.xlsx
+++ b/data/metrics/sens.filt.2020-12-23.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\LGSS_scripting\lgss\data\metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BE88A0F-254C-4E00-8DFA-FDB261F97067}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C7081CB-AB10-41B3-A237-6BFB463A697B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-5895" yWindow="3720" windowWidth="12945" windowHeight="15300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12540" yWindow="765" windowWidth="15180" windowHeight="15300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sens.filt.2020-12-23" sheetId="1" r:id="rId1"/>
@@ -1169,7 +1169,7 @@
   <dimension ref="A1:K37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:H4"/>
+      <selection activeCell="B19" sqref="B19:E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1304,66 +1304,60 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D5" t="s">
-        <v>48</v>
+        <v>39</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="E5" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="F5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G5">
-        <v>3.2795698924731198</v>
+        <v>12.802199860946899</v>
       </c>
       <c r="H5">
-        <v>66.6666666666667</v>
+        <v>83.3333333333333</v>
       </c>
       <c r="I5">
-        <v>3.0913043478260902</v>
+        <v>12.1603274157769</v>
       </c>
       <c r="J5">
-        <v>70.483870967741893</v>
+        <v>81.989247311827995</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="B6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>33</v>
-      </c>
-      <c r="D6" t="s">
-        <v>60</v>
       </c>
       <c r="E6" t="s">
         <v>8</v>
       </c>
       <c r="F6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G6">
-        <v>18.452380952380999</v>
+        <v>2.1485946181198501</v>
       </c>
       <c r="H6">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="I6">
-        <v>19.5299145299145</v>
+        <v>2.0499744890133198</v>
       </c>
       <c r="J6">
-        <v>70.483870967741893</v>
+        <v>80.322580645161295</v>
       </c>
       <c r="K6" s="4"/>
     </row>
@@ -1371,46 +1365,46 @@
       <c r="A7" t="s">
         <v>47</v>
       </c>
-      <c r="B7" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>65</v>
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" t="s">
+        <v>33</v>
       </c>
       <c r="D7" t="s">
-        <v>73</v>
+        <v>48</v>
       </c>
       <c r="E7" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="F7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G7">
-        <v>22.835497835497801</v>
+        <v>3.2795698924731198</v>
       </c>
       <c r="H7">
-        <v>80</v>
+        <v>66.6666666666667</v>
       </c>
       <c r="I7">
-        <v>21.506513409961698</v>
+        <v>3.0913043478260902</v>
       </c>
       <c r="J7">
-        <v>75.430107526881699</v>
+        <v>70.483870967741893</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>47</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>50</v>
+      <c r="B8" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>65</v>
       </c>
       <c r="D8" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E8" t="s">
         <v>8</v>
@@ -1425,10 +1419,10 @@
         <v>80</v>
       </c>
       <c r="I8">
-        <v>21.269509981851201</v>
+        <v>21.506513409961698</v>
       </c>
       <c r="J8">
-        <v>80.268817204301101</v>
+        <v>75.430107526881699</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -1436,45 +1430,45 @@
         <v>47</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>54</v>
       </c>
       <c r="C9" t="s">
         <v>33</v>
       </c>
       <c r="D9" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="E9" t="s">
         <v>8</v>
       </c>
       <c r="F9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G9">
-        <v>15.470494417862801</v>
+        <v>18.452380952380999</v>
       </c>
       <c r="H9">
-        <v>76.6666666666667</v>
+        <v>70</v>
       </c>
       <c r="I9">
-        <v>15.6785714285714</v>
+        <v>19.5299145299145</v>
       </c>
       <c r="J9">
-        <v>75.430107526881699</v>
+        <v>70.483870967741893</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>40</v>
-      </c>
-      <c r="B10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" t="s">
-        <v>33</v>
+        <v>47</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>50</v>
       </c>
       <c r="D10" t="s">
-        <v>45</v>
+        <v>71</v>
       </c>
       <c r="E10" t="s">
         <v>8</v>
@@ -1483,30 +1477,30 @@
         <v>3</v>
       </c>
       <c r="G10">
-        <v>15.5</v>
+        <v>22.835497835497801</v>
       </c>
       <c r="H10">
         <v>80</v>
       </c>
       <c r="I10">
-        <v>15.14</v>
+        <v>21.269509981851201</v>
       </c>
       <c r="J10">
-        <v>77.096774193548399</v>
+        <v>80.268817204301101</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C11" t="s">
         <v>33</v>
       </c>
       <c r="D11" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="E11" t="s">
         <v>8</v>
@@ -1515,30 +1509,30 @@
         <v>3</v>
       </c>
       <c r="G11">
-        <v>30</v>
+        <v>15.470494417862801</v>
       </c>
       <c r="H11">
-        <v>80</v>
+        <v>76.6666666666667</v>
       </c>
       <c r="I11">
-        <v>29.88</v>
+        <v>15.6785714285714</v>
       </c>
       <c r="J11">
-        <v>78.709677419354804</v>
+        <v>75.430107526881699</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>40</v>
       </c>
-      <c r="B12" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>68</v>
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" t="s">
+        <v>45</v>
       </c>
       <c r="E12" t="s">
         <v>8</v>
@@ -1547,16 +1541,16 @@
         <v>3</v>
       </c>
       <c r="G12">
-        <v>30.5</v>
+        <v>15.5</v>
       </c>
       <c r="H12">
-        <v>83.3333333333333</v>
+        <v>80</v>
       </c>
       <c r="I12">
-        <v>29.6</v>
+        <v>15.14</v>
       </c>
       <c r="J12">
-        <v>80.322580645161295</v>
+        <v>77.096774193548399</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -1564,234 +1558,237 @@
         <v>40</v>
       </c>
       <c r="B13" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="C13" t="s">
         <v>33</v>
       </c>
       <c r="D13" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E13" t="s">
         <v>8</v>
       </c>
       <c r="F13">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G13">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="H13">
-        <v>66.6666666666667</v>
+        <v>80</v>
       </c>
       <c r="I13">
-        <v>7</v>
+        <v>29.88</v>
       </c>
       <c r="J13">
-        <v>65.591397849462396</v>
+        <v>78.709677419354804</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>40</v>
       </c>
-      <c r="B14" t="s">
-        <v>29</v>
-      </c>
-      <c r="C14" t="s">
-        <v>33</v>
-      </c>
-      <c r="D14" t="s">
-        <v>51</v>
+      <c r="B14" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>68</v>
       </c>
       <c r="E14" t="s">
         <v>8</v>
       </c>
       <c r="F14">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G14">
-        <v>11.5</v>
+        <v>30.5</v>
       </c>
       <c r="H14">
-        <v>66.6666666666667</v>
+        <v>83.3333333333333</v>
       </c>
       <c r="I14">
-        <v>11.68</v>
+        <v>29.6</v>
       </c>
       <c r="J14">
-        <v>70.430107526881699</v>
+        <v>80.322580645161295</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>40</v>
       </c>
-      <c r="B15" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>34</v>
+      <c r="B15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" t="s">
+        <v>33</v>
       </c>
       <c r="D15" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="E15" t="s">
         <v>8</v>
       </c>
       <c r="F15">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G15">
-        <v>3.5</v>
+        <v>11.5</v>
       </c>
       <c r="H15">
-        <v>86.6666666666667</v>
+        <v>66.6666666666667</v>
       </c>
       <c r="I15">
-        <v>2.6</v>
+        <v>11.68</v>
       </c>
       <c r="J15">
-        <v>83.494623655913998</v>
+        <v>70.430107526881699</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>40</v>
       </c>
-      <c r="B16" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>53</v>
+      <c r="B16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" t="s">
+        <v>33</v>
       </c>
       <c r="D16" t="s">
-        <v>69</v>
+        <v>44</v>
       </c>
       <c r="E16" t="s">
         <v>8</v>
       </c>
       <c r="F16">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G16">
-        <v>3.5</v>
+        <v>7</v>
       </c>
       <c r="H16">
-        <v>86.6666666666667</v>
+        <v>66.6666666666667</v>
       </c>
       <c r="I16">
-        <v>2.6</v>
+        <v>7</v>
       </c>
       <c r="J16">
-        <v>83.494623655913998</v>
+        <v>65.591397849462396</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>42</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="C17" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="7" t="s">
         <v>34</v>
       </c>
       <c r="D17" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="E17" t="s">
         <v>8</v>
       </c>
       <c r="F17">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G17">
-        <v>10.5</v>
+        <v>3.5</v>
       </c>
       <c r="H17">
-        <v>66.6666666666667</v>
+        <v>86.6666666666667</v>
       </c>
       <c r="I17">
-        <v>11.4</v>
+        <v>2.6</v>
       </c>
       <c r="J17">
-        <v>65.591397849462396</v>
+        <v>83.494623655913998</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>46</v>
-      </c>
-      <c r="B18" t="s">
-        <v>27</v>
-      </c>
-      <c r="C18" t="s">
-        <v>33</v>
+        <v>40</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D18" t="s">
+        <v>69</v>
       </c>
       <c r="E18" t="s">
         <v>8</v>
       </c>
       <c r="F18">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G18">
-        <v>2.8084333787031799</v>
+        <v>3.5</v>
       </c>
       <c r="H18">
-        <v>66.6666666666667</v>
+        <v>86.6666666666667</v>
       </c>
       <c r="I18">
-        <v>2.9091287722608201</v>
+        <v>2.6</v>
       </c>
       <c r="J18">
-        <v>70.483870967741893</v>
+        <v>83.494623655913998</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>46</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C19" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>34</v>
       </c>
       <c r="D19" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="E19" t="s">
         <v>8</v>
       </c>
       <c r="F19">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G19">
-        <v>19</v>
+        <v>10.5</v>
       </c>
       <c r="H19">
-        <v>76.6666666666667</v>
+        <v>66.6666666666667</v>
       </c>
       <c r="I19">
-        <v>18.86</v>
+        <v>11.4</v>
       </c>
       <c r="J19">
-        <v>77.043010752688204</v>
+        <v>65.591397849462396</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>46</v>
       </c>
-      <c r="B20" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>35</v>
+      <c r="B20" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>34</v>
       </c>
       <c r="D20" t="s">
-        <v>52</v>
+        <v>72</v>
       </c>
       <c r="E20" t="s">
         <v>8</v>
@@ -1800,13 +1797,13 @@
         <v>3</v>
       </c>
       <c r="G20">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="H20">
         <v>76.6666666666667</v>
       </c>
       <c r="I20">
-        <v>2.46</v>
+        <v>18.86</v>
       </c>
       <c r="J20">
         <v>77.043010752688204</v>
@@ -1816,87 +1813,93 @@
       <c r="A21" t="s">
         <v>46</v>
       </c>
-      <c r="B21" t="s">
-        <v>21</v>
-      </c>
-      <c r="C21" t="s">
-        <v>33</v>
+      <c r="B21" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D21" t="s">
+        <v>52</v>
       </c>
       <c r="E21" t="s">
         <v>8</v>
       </c>
       <c r="F21">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G21">
-        <v>2.8742545493052498</v>
+        <v>3</v>
       </c>
       <c r="H21">
-        <v>73.3333333333333</v>
+        <v>76.6666666666667</v>
       </c>
       <c r="I21">
-        <v>2.8900060206038201</v>
+        <v>2.46</v>
       </c>
       <c r="J21">
-        <v>73.763440860214999</v>
+        <v>77.043010752688204</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>39</v>
       </c>
-      <c r="B22" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>35</v>
+      <c r="B22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="E22" t="s">
         <v>8</v>
       </c>
       <c r="F22">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G22">
-        <v>12.802199860946899</v>
+        <v>3.5195695769510902</v>
       </c>
       <c r="H22">
-        <v>83.3333333333333</v>
+        <v>70</v>
       </c>
       <c r="I22">
-        <v>12.1603274157769</v>
+        <v>3.6086681021069298</v>
       </c>
       <c r="J22">
-        <v>81.989247311827995</v>
+        <v>72.150537634408593</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>39</v>
       </c>
-      <c r="B23" t="s">
-        <v>11</v>
+      <c r="B23" s="4" t="s">
+        <v>55</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E23" t="s">
+      <c r="D23" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E23" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="4">
         <v>3</v>
       </c>
-      <c r="G23">
-        <v>2.1485946181198501</v>
-      </c>
-      <c r="H23">
-        <v>80</v>
-      </c>
-      <c r="I23">
-        <v>2.0499744890133198</v>
-      </c>
-      <c r="J23">
-        <v>80.322580645161295</v>
+      <c r="G23" s="4">
+        <v>1.8373207647735701</v>
+      </c>
+      <c r="H23" s="4">
+        <v>76.6666666666667</v>
+      </c>
+      <c r="I23" s="4">
+        <v>1.8155980723852001</v>
+      </c>
+      <c r="J23" s="4">
+        <v>77.043010752688204</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -1904,7 +1907,7 @@
         <v>39</v>
       </c>
       <c r="B24" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>33</v>
@@ -1913,173 +1916,170 @@
         <v>8</v>
       </c>
       <c r="F24">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G24">
-        <v>3.5195695769510902</v>
+        <v>1.78284002465393</v>
       </c>
       <c r="H24">
-        <v>70</v>
+        <v>76.6666666666667</v>
       </c>
       <c r="I24">
-        <v>3.6086681021069298</v>
+        <v>1.79280681362995</v>
       </c>
       <c r="J24">
-        <v>72.150537634408593</v>
+        <v>77.096774193548399</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>39</v>
       </c>
-      <c r="B25" t="s">
-        <v>16</v>
+      <c r="B25" s="4" t="s">
+        <v>56</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E25" t="s">
+      <c r="D25" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E25" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="4">
         <v>3</v>
       </c>
-      <c r="G25">
-        <v>1.78284002465393</v>
-      </c>
-      <c r="H25">
-        <v>76.6666666666667</v>
-      </c>
-      <c r="I25">
-        <v>1.79280681362995</v>
-      </c>
-      <c r="J25">
-        <v>77.096774193548399</v>
+      <c r="G25" s="4">
+        <v>2.1209372298772502</v>
+      </c>
+      <c r="H25" s="4">
+        <v>86.6666666666667</v>
+      </c>
+      <c r="I25" s="4">
+        <v>1.8608292713544801</v>
+      </c>
+      <c r="J25" s="4">
+        <v>80.322580645161295</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>39</v>
       </c>
-      <c r="B26" t="s">
-        <v>28</v>
+      <c r="B26" s="4" t="s">
+        <v>57</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E26" t="s">
+      <c r="D26" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E26" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F26">
-        <v>2</v>
-      </c>
-      <c r="G26">
-        <v>3.4424427630108601</v>
-      </c>
-      <c r="H26">
-        <v>70</v>
-      </c>
-      <c r="I26">
-        <v>3.4442082477334099</v>
-      </c>
-      <c r="J26">
-        <v>70.483870967741893</v>
+      <c r="F26" s="4">
+        <v>3</v>
+      </c>
+      <c r="G26" s="4">
+        <v>1.8528303225668401</v>
+      </c>
+      <c r="H26" s="4">
+        <v>83.3333333333333</v>
+      </c>
+      <c r="I26" s="4">
+        <v>1.6145410757637799</v>
+      </c>
+      <c r="J26" s="4">
+        <v>83.602150537634401</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>39</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C27" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B27" t="s">
+        <v>27</v>
+      </c>
+      <c r="C27" t="s">
         <v>33</v>
       </c>
-      <c r="D27" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E27" s="4" t="s">
+      <c r="E27" t="s">
         <v>8</v>
       </c>
-      <c r="F27" s="4">
-        <v>3</v>
-      </c>
-      <c r="G27" s="4">
-        <v>1.8373207647735701</v>
-      </c>
-      <c r="H27" s="4">
-        <v>76.6666666666667</v>
-      </c>
-      <c r="I27" s="4">
-        <v>1.8155980723852001</v>
-      </c>
-      <c r="J27" s="4">
-        <v>77.043010752688204</v>
+      <c r="F27">
+        <v>2</v>
+      </c>
+      <c r="G27">
+        <v>2.8084333787031799</v>
+      </c>
+      <c r="H27">
+        <v>66.6666666666667</v>
+      </c>
+      <c r="I27">
+        <v>2.9091287722608201</v>
+      </c>
+      <c r="J27">
+        <v>70.483870967741893</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>39</v>
       </c>
-      <c r="B28" s="4" t="s">
-        <v>56</v>
+      <c r="B28" t="s">
+        <v>28</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D28" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="E28" s="4" t="s">
+      <c r="E28" t="s">
         <v>8</v>
       </c>
-      <c r="F28" s="4">
-        <v>3</v>
-      </c>
-      <c r="G28" s="4">
-        <v>2.1209372298772502</v>
-      </c>
-      <c r="H28" s="4">
-        <v>86.6666666666667</v>
-      </c>
-      <c r="I28" s="4">
-        <v>1.8608292713544801</v>
-      </c>
-      <c r="J28" s="4">
-        <v>80.322580645161295</v>
+      <c r="F28">
+        <v>2</v>
+      </c>
+      <c r="G28">
+        <v>3.4424427630108601</v>
+      </c>
+      <c r="H28">
+        <v>70</v>
+      </c>
+      <c r="I28">
+        <v>3.4442082477334099</v>
+      </c>
+      <c r="J28">
+        <v>70.483870967741893</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>39</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C29" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B29" t="s">
+        <v>21</v>
+      </c>
+      <c r="C29" t="s">
         <v>33</v>
       </c>
-      <c r="D29" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E29" s="4" t="s">
+      <c r="E29" t="s">
         <v>8</v>
       </c>
-      <c r="F29" s="4">
-        <v>3</v>
-      </c>
-      <c r="G29" s="4">
-        <v>1.8528303225668401</v>
-      </c>
-      <c r="H29" s="4">
-        <v>83.3333333333333</v>
-      </c>
-      <c r="I29" s="4">
-        <v>1.6145410757637799</v>
-      </c>
-      <c r="J29" s="4">
-        <v>83.602150537634401</v>
+      <c r="F29">
+        <v>2</v>
+      </c>
+      <c r="G29">
+        <v>2.8742545493052498</v>
+      </c>
+      <c r="H29">
+        <v>73.3333333333333</v>
+      </c>
+      <c r="I29">
+        <v>2.8900060206038201</v>
+      </c>
+      <c r="J29">
+        <v>73.763440860214999</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
@@ -2150,28 +2150,31 @@
       <c r="A32" t="s">
         <v>39</v>
       </c>
-      <c r="B32" t="s">
-        <v>23</v>
+      <c r="B32" s="4" t="s">
+        <v>61</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E32" t="s">
+      <c r="D32" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E32" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F32">
+      <c r="F32" s="4">
         <v>2</v>
       </c>
-      <c r="G32">
-        <v>0.371111111111111</v>
-      </c>
-      <c r="H32">
+      <c r="G32" s="4">
+        <v>0.34647433758789498</v>
+      </c>
+      <c r="H32" s="4">
         <v>70</v>
       </c>
-      <c r="I32">
-        <v>0.33212144116906001</v>
-      </c>
-      <c r="J32">
+      <c r="I32" s="4">
+        <v>0.32888888888888901</v>
+      </c>
+      <c r="J32" s="4">
         <v>72.150537634408593</v>
       </c>
     </row>
@@ -2179,31 +2182,28 @@
       <c r="A33" t="s">
         <v>39</v>
       </c>
-      <c r="B33" s="4" t="s">
-        <v>61</v>
+      <c r="B33" t="s">
+        <v>23</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D33" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E33" s="4" t="s">
+      <c r="E33" t="s">
         <v>24</v>
       </c>
-      <c r="F33" s="4">
+      <c r="F33">
         <v>2</v>
       </c>
-      <c r="G33" s="4">
-        <v>0.34647433758789498</v>
-      </c>
-      <c r="H33" s="4">
+      <c r="G33">
+        <v>0.371111111111111</v>
+      </c>
+      <c r="H33">
         <v>70</v>
       </c>
-      <c r="I33" s="4">
-        <v>0.32888888888888901</v>
-      </c>
-      <c r="J33" s="4">
+      <c r="I33">
+        <v>0.33212144116906001</v>
+      </c>
+      <c r="J33">
         <v>72.150537634408593</v>
       </c>
     </row>
@@ -2307,10 +2307,8 @@
       <c r="D37" s="4"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:J32">
-    <sortCondition ref="B2:B32"/>
-    <sortCondition ref="H2:H32"/>
-    <sortCondition ref="F2:F32"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J36">
+    <sortCondition ref="B6"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>